<commit_message>
Save payment_info to xlsx file
</commit_message>
<xml_diff>
--- a/payment_info.xlsx
+++ b/payment_info.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +412,28 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="8.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13.140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="23.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="15.5703125" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="28.140625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="13.140625" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="12.42578125" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="11.28515625" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" min="10" max="11"/>
+    <col width="10.140625" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="48.28515625" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="31.28515625" bestFit="1" customWidth="1" min="14" max="14"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -630,6 +644,146 @@
       <c r="N3" t="inlineStr">
         <is>
           <t>ch_3PA6NxBSTDzLM9dR0ZFsfW7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>phone1 (45), phone2 (55)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>380951075000</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>bbtxdbnbxbfgnb@gmailc.com</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>RU</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>trthrdytfuyjh</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>rtdfygjuhjkl</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>agshdjyfkhj</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>sdtfygjuhkj</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>6847373164_539544748_60970_7362462363001257276</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>ch_3PA6i1BSTDzLM9dR2xLrLp4H</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>59</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>monitor5 (59)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>85225685556</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>hcyxtdy@gmail.com</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>BN</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Омнсгсгпщ</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Дмлмшмдп</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Момшпшп</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Шпшпгмг</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>457</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>6847373164_698774231_162277_7362581855223546880</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>ch_3PAE0sBSTDzLM9dR2qEDltOJ</t>
         </is>
       </c>
     </row>

</xml_diff>